<commit_message>
Só deixar alterar a avaliação no maximo duas vezes
</commit_message>
<xml_diff>
--- a/ExperimentoLinguistica/wwwroot/resultado_avaliacao.xlsx
+++ b/ExperimentoLinguistica/wwwroot/resultado_avaliacao.xlsx
@@ -3,19 +3,25 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27830"/>
   <workbookPr defaultThemeVersion="202300"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\raphael.pinheiro\source\repos\ExperimentoLinguistica\ExperimentoLinguistica\wwwroot\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BA0213B6-DD9B-4FF6-8D00-12242A90BE37}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-84" yWindow="12852" windowWidth="23256" windowHeight="12576"/>
+    <workbookView xWindow="-84" yWindow="12852" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Planilha1" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
-    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
-      <x15:workbookPr xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" chartTrackingRefBase="1"/>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+      <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
-    <ext uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures">
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
         <xcalcf:feature name="microsoft.com:RD"/>
         <xcalcf:feature name="microsoft.com:Single"/>
         <xcalcf:feature name="microsoft.com:FV"/>
@@ -30,52 +36,51 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="13">
-  <si>
-    <t xml:space="preserve">IdPessoa</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Prime</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Alvo</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Avaliacao</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Lista</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Idioma</t>
-  </si>
-  <si>
-    <t xml:space="preserve">939449fc-e922-08dc-85ef-6ac73a4120ae</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Japones</t>
-  </si>
-  <si>
-    <t xml:space="preserve">B</t>
-  </si>
-  <si>
-    <t xml:space="preserve">苹果</t>
-  </si>
-  <si>
-    <t xml:space="preserve">pincel</t>
-  </si>
-  <si>
-    <t xml:space="preserve">没关系</t>
-  </si>
-  <si>
-    <t xml:space="preserve">jaddkks</t>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="13">
+  <si>
+    <t>IdPessoa</t>
+  </si>
+  <si>
+    <t>Prime</t>
+  </si>
+  <si>
+    <t>Alvo</t>
+  </si>
+  <si>
+    <t>Avaliacao</t>
+  </si>
+  <si>
+    <t>Lista</t>
+  </si>
+  <si>
+    <t>Idioma</t>
+  </si>
+  <si>
+    <t>939449fc-e922-08dc-85ef-6ac73a4120ae</t>
+  </si>
+  <si>
+    <t>Japones</t>
+  </si>
+  <si>
+    <t>B</t>
+  </si>
+  <si>
+    <t>苹果</t>
+  </si>
+  <si>
+    <t>pincel</t>
+  </si>
+  <si>
+    <t>没关系</t>
+  </si>
+  <si>
+    <t>jaddkks</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="0"/>
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -114,11 +119,11 @@
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
-    <ext uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
-      <x14:slicerStyles xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" defaultSlicerStyle="SlicerStyleLight1"/>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
     </ext>
-    <ext uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
-      <x15:timelineStyles xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
     </ext>
   </extLst>
 </styleSheet>
@@ -412,7 +417,7 @@
   <a:objectDefaults>
     <a:lnDef>
       <a:spPr/>
-      <a:bodyPr rtlCol="0"/>
+      <a:bodyPr/>
       <a:lstStyle/>
       <a:style>
         <a:lnRef idx="2">
@@ -440,216 +445,79 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3">
-  <dimension ref="A1:G10"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:F3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G5" sqref="G5"/>
+      <selection activeCell="F20" sqref="A4:F20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="30.28515625" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A1" s="0" t="s">
+      <c r="A1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="0" t="s">
+      <c r="B1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="0" t="s">
+      <c r="C1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="0" t="s">
+      <c r="D1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="0" t="s">
+      <c r="E1" t="s">
         <v>5</v>
       </c>
-      <c r="F1" s="0" t="s">
+      <c r="F1" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="2">
-      <c r="A2" s="0" t="s">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
         <v>6</v>
       </c>
-      <c r="B2" s="0" t="s">
+      <c r="B2" t="s">
         <v>7</v>
       </c>
-      <c r="C2" s="0" t="s">
+      <c r="C2" t="s">
         <v>8</v>
       </c>
-      <c r="D2" s="0" t="s">
+      <c r="D2" t="s">
         <v>9</v>
       </c>
-      <c r="E2" s="0" t="s">
+      <c r="E2" t="s">
         <v>10</v>
       </c>
-      <c r="F2" s="0">
+      <c r="F2">
         <v>4</v>
       </c>
     </row>
-    <row r="3">
-      <c r="A3" s="0" t="s">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
         <v>6</v>
       </c>
-      <c r="B3" s="0" t="s">
+      <c r="B3" t="s">
         <v>7</v>
       </c>
-      <c r="C3" s="0" t="s">
+      <c r="C3" t="s">
         <v>8</v>
       </c>
-      <c r="D3" s="0" t="s">
+      <c r="D3" t="s">
         <v>11</v>
       </c>
-      <c r="E3" s="0" t="s">
+      <c r="E3" t="s">
         <v>12</v>
       </c>
-      <c r="F3" s="0">
+      <c r="F3">
         <v>3</v>
-      </c>
-    </row>
-    <row r="4">
-      <c r="A4" s="0" t="s">
-        <v>6</v>
-      </c>
-      <c r="B4" s="0" t="s">
-        <v>9</v>
-      </c>
-      <c r="C4" s="0" t="s">
-        <v>10</v>
-      </c>
-      <c r="D4" s="0">
-        <v>2</v>
-      </c>
-      <c r="E4" s="0" t="s">
-        <v>7</v>
-      </c>
-      <c r="F4" s="0" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="5">
-      <c r="A5" s="0" t="s">
-        <v>6</v>
-      </c>
-      <c r="B5" s="0" t="s">
-        <v>11</v>
-      </c>
-      <c r="C5" s="0" t="s">
-        <v>12</v>
-      </c>
-      <c r="D5" s="0">
-        <v>4</v>
-      </c>
-      <c r="E5" s="0" t="s">
-        <v>7</v>
-      </c>
-      <c r="F5" s="0" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="6">
-      <c r="A6" s="0" t="s">
-        <v>6</v>
-      </c>
-      <c r="B6" s="0" t="s">
-        <v>9</v>
-      </c>
-      <c r="C6" s="0" t="s">
-        <v>10</v>
-      </c>
-      <c r="D6" s="0">
-        <v>1</v>
-      </c>
-      <c r="E6" s="0" t="s">
-        <v>7</v>
-      </c>
-      <c r="F6" s="0" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="7">
-      <c r="A7" s="0" t="s">
-        <v>6</v>
-      </c>
-      <c r="B7" s="0" t="s">
-        <v>9</v>
-      </c>
-      <c r="C7" s="0" t="s">
-        <v>10</v>
-      </c>
-      <c r="D7" s="0">
-        <v>5</v>
-      </c>
-      <c r="E7" s="0" t="s">
-        <v>7</v>
-      </c>
-      <c r="F7" s="0" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="8">
-      <c r="A8" s="0" t="s">
-        <v>6</v>
-      </c>
-      <c r="B8" s="0" t="s">
-        <v>9</v>
-      </c>
-      <c r="C8" s="0" t="s">
-        <v>10</v>
-      </c>
-      <c r="D8" s="0">
-        <v>4</v>
-      </c>
-      <c r="E8" s="0" t="s">
-        <v>7</v>
-      </c>
-      <c r="F8" s="0" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="9">
-      <c r="A9" s="0" t="s">
-        <v>6</v>
-      </c>
-      <c r="B9" s="0" t="s">
-        <v>9</v>
-      </c>
-      <c r="C9" s="0" t="s">
-        <v>10</v>
-      </c>
-      <c r="D9" s="0">
-        <v>2</v>
-      </c>
-      <c r="E9" s="0" t="s">
-        <v>7</v>
-      </c>
-      <c r="F9" s="0" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="10">
-      <c r="A10" s="0" t="s">
-        <v>6</v>
-      </c>
-      <c r="B10" s="0" t="s">
-        <v>9</v>
-      </c>
-      <c r="C10" s="0" t="s">
-        <v>10</v>
-      </c>
-      <c r="D10" s="0">
-        <v>5</v>
-      </c>
-      <c r="E10" s="0" t="s">
-        <v>7</v>
-      </c>
-      <c r="F10" s="0" t="s">
-        <v>8</v>
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.511811024" right="0.511811024" top="0.787401575" bottom="0.787401575" header="0.31496062" footer="0.31496062"/>
+  <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
 </worksheet>
 </file>
</xml_diff>